<commit_message>
Themenaingabe angepasst, TODOs ergänzt
</commit_message>
<xml_diff>
--- a/Planung/TODOS.xlsx
+++ b/Planung/TODOS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Was</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Template für Artefaktmigration erstellen</t>
+  </si>
+  <si>
+    <t>Themeneingabe Planung/Deliverables/etc. anpassen??</t>
   </si>
 </sst>
 </file>
@@ -470,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -569,56 +572,61 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+    <row r="17" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+    <row r="21" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Vorlage Aspektbearbeitung, Statusbericht, diverse Updates
</commit_message>
<xml_diff>
--- a/Planung/TODOS.xlsx
+++ b/Planung/TODOS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Was</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Themeneingabe Planung/Deliverables/etc. anpassen??</t>
+  </si>
+  <si>
+    <t>Alle Templates harmonisieren</t>
+  </si>
+  <si>
+    <t>Bericht</t>
   </si>
 </sst>
 </file>
@@ -164,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -172,6 +178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -473,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -590,44 +597,57 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="5">
+        <v>41518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>